<commit_message>
Adding fields on detail screen. Improve code
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Version</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Improve code</t>
+  </si>
+  <si>
+    <t>Adding field on detail screen, improve code</t>
   </si>
 </sst>
 </file>
@@ -463,7 +466,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
@@ -555,6 +558,23 @@
         <v>8</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>43653</v>
+      </c>
+      <c r="B6" s="5">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="7">
+        <v>4</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:D1"/>

</xml_diff>